<commit_message>
Formulas fix, more examples
</commit_message>
<xml_diff>
--- a/XlsSerializer.Examples.Web/data/Xlsx/CellLabels.xlsx
+++ b/XlsSerializer.Examples.Web/data/Xlsx/CellLabels.xlsx
@@ -17,10 +17,10 @@
     <t>First Label</t>
   </si>
   <si>
-    <t>bc74e581-d020-4450-87ad-136760f9f662</t>
+    <t>8154b3c0-4152-4a08-811e-2c2837f14d24</t>
   </si>
   <si>
-    <t>7ce069ed-098a-4110-8c81-953a6c354751</t>
+    <t>51cc4521-b585-476b-b67d-9dd0425fd5dd</t>
   </si>
 </sst>
 </file>

</xml_diff>